<commit_message>
v1.1: Improved visualisation readability
</commit_message>
<xml_diff>
--- a/data/exampledata.xlsx
+++ b/data/exampledata.xlsx
@@ -44,9 +44,6 @@
     <t>Manchester</t>
   </si>
   <si>
-    <t>MS</t>
-  </si>
-  <si>
     <t>Digital</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>Sheffield</t>
+  </si>
+  <si>
+    <t>Musculoskeletal</t>
   </si>
 </sst>
 </file>
@@ -377,10 +377,13 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A33"/>
+      <selection activeCell="C18" sqref="C18:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -390,7 +393,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -407,10 +410,10 @@
         <v>2017</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -424,10 +427,10 @@
         <v>2016</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>17</v>
@@ -441,10 +444,10 @@
         <v>2015</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4">
         <v>13</v>
@@ -458,10 +461,10 @@
         <v>2014</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -469,16 +472,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>2017</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <v>13</v>
@@ -486,16 +489,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>2016</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -503,16 +506,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>2015</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8">
         <v>11</v>
@@ -520,16 +523,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>2014</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -543,10 +546,10 @@
         <v>2017</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10">
         <v>20</v>
@@ -560,10 +563,10 @@
         <v>2016</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11">
         <v>17</v>
@@ -577,10 +580,10 @@
         <v>2015</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12">
         <v>13</v>
@@ -594,10 +597,10 @@
         <v>2014</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -605,16 +608,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14">
         <v>2017</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14">
         <v>13</v>
@@ -622,16 +625,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <v>2016</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15">
         <v>12</v>
@@ -639,16 +642,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <v>2015</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16">
         <v>11</v>
@@ -656,16 +659,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>2014</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17">
         <v>10</v>
@@ -679,10 +682,10 @@
         <v>2017</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18">
         <v>17</v>
@@ -696,10 +699,10 @@
         <v>2016</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19">
         <v>14</v>
@@ -713,10 +716,10 @@
         <v>2015</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E20">
         <v>15</v>
@@ -730,10 +733,10 @@
         <v>2014</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E21">
         <v>18</v>
@@ -741,16 +744,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22">
         <v>2017</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E22">
         <v>12</v>
@@ -758,16 +761,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23">
         <v>2016</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E23">
         <v>11</v>
@@ -775,16 +778,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24">
         <v>2015</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24">
         <v>13</v>
@@ -792,16 +795,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25">
         <v>2014</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E25">
         <v>12</v>
@@ -809,16 +812,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26">
         <v>2017</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E26">
         <v>28</v>
@@ -826,16 +829,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27">
         <v>2016</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E27">
         <v>26</v>
@@ -843,16 +846,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28">
         <v>2015</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28">
         <v>24</v>
@@ -860,16 +863,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29">
         <v>2014</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E29">
         <v>22</v>
@@ -883,10 +886,10 @@
         <v>2017</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E30">
         <v>17</v>
@@ -900,10 +903,10 @@
         <v>2016</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31">
         <v>15</v>
@@ -917,10 +920,10 @@
         <v>2015</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E32">
         <v>13</v>
@@ -934,10 +937,10 @@
         <v>2014</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E33">
         <v>11</v>

</xml_diff>